<commit_message>
Add random username and email generator
</commit_message>
<xml_diff>
--- a/Test Cases BB.xlsx
+++ b/Test Cases BB.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christine.onyango/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christine.onyango/Documents/backbase-assignment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40946E7A-F636-5C4C-9688-A2608FC7E617}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EA94A51-C2BF-984C-A17C-E2300FBE21F5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{1633F945-08CF-F441-8B67-BD8C983AE1BC}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18900" xr2:uid="{1633F945-08CF-F441-8B67-BD8C983AE1BC}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="122">
   <si>
     <t>Test Case</t>
   </si>
@@ -182,18 +182,6 @@
   </si>
   <si>
     <t>This is a design enhancement that would make the app more usable in addition to having proper labels on the login fields</t>
-  </si>
-  <si>
-    <t>Form field labels</t>
-  </si>
-  <si>
-    <t>All form fields should be labelled accordingly</t>
-  </si>
-  <si>
-    <t>Verify that form fields are labelled accordingly</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Form fields are not labelled. Placeholders do not suffice as they cease to be visible once a user starts typing in </t>
   </si>
   <si>
     <t>Registration</t>
@@ -925,10 +913,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{244B7FE0-D1F2-7A43-BD54-E16A5E9DC925}">
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1038,7 +1026,7 @@
         <v>14</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>28</v>
@@ -1058,7 +1046,7 @@
         <v>15</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>32</v>
@@ -1109,189 +1097,189 @@
     </row>
     <row r="9" spans="1:9" ht="51">
       <c r="C9" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="H9" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="136">
+    <row r="10" spans="1:9" ht="102">
       <c r="C10" s="1" t="s">
-        <v>43</v>
+        <v>87</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>45</v>
+        <v>89</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>90</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>44</v>
+        <v>91</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>46</v>
+        <v>88</v>
       </c>
       <c r="H10" s="5" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" ht="102">
+      <c r="I10" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="68">
       <c r="C11" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="D11" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="E11" s="3"/>
+      <c r="F11" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="I11" s="1"/>
+    </row>
+    <row r="12" spans="1:9" ht="153">
+      <c r="A12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="F12" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="187">
+      <c r="C13" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="204">
+      <c r="C14" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="170">
+      <c r="C15" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="E15" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="G11" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="H11" s="5" t="s">
+      <c r="F15" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="119">
+      <c r="C16" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H16" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="I11" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="68">
-      <c r="C12" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="E12" s="3"/>
-      <c r="F12" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="H12" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="I12" s="1"/>
-    </row>
-    <row r="13" spans="1:9" ht="153">
-      <c r="A13" t="s">
-        <v>47</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="E13" s="1" t="s">
+    </row>
+    <row r="17" spans="1:9" ht="102">
+      <c r="C17" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="F13" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="187">
-      <c r="C14" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="204">
-      <c r="C15" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E15" s="1" t="s">
+      <c r="F17" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G17" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="F15" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="170">
-      <c r="C16" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="H16" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="119">
-      <c r="C17" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="H17" s="5" t="s">
-        <v>30</v>
+      <c r="H17" s="4" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="102">
       <c r="C18" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="H18" s="4" t="s">
         <v>21</v>
@@ -1299,126 +1287,109 @@
     </row>
     <row r="19" spans="1:9" ht="102">
       <c r="C19" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H19" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="102">
+    <row r="20" spans="1:9" ht="85">
+      <c r="A20" t="s">
+        <v>82</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>107</v>
+      </c>
       <c r="C20" s="1" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="D20" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="170">
+      <c r="C21" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="F20" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="H20" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="85">
-      <c r="A21" t="s">
-        <v>86</v>
-      </c>
-      <c r="B21" s="1" t="s">
+      <c r="D21" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="153">
+      <c r="A22" t="s">
+        <v>112</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="170">
+      <c r="C23" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H23" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="H21" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="170">
-      <c r="C22" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="H22" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="153">
-      <c r="A23" t="s">
+      <c r="I23" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="H23" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="170">
+    </row>
+    <row r="24" spans="1:9" ht="51" hidden="1">
       <c r="C24" s="1" t="s">
         <v>117</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>118</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="H24" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="51" hidden="1">
-      <c r="C25" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>122</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" xr:uid="{A899D309-FAAF-C145-855C-424A9DF8EAC7}"/>
-    <hyperlink ref="E11" r:id="rId2" display="TINAONYANGO@GMAIL.COM" xr:uid="{569523E9-BA31-F443-B30B-74466176CE2B}"/>
-    <hyperlink ref="E16" r:id="rId3" xr:uid="{CAC9AD4E-C9D1-5642-8071-EB1356541E8F}"/>
+    <hyperlink ref="E10" r:id="rId2" display="TINAONYANGO@GMAIL.COM" xr:uid="{569523E9-BA31-F443-B30B-74466176CE2B}"/>
+    <hyperlink ref="E15" r:id="rId3" xr:uid="{CAC9AD4E-C9D1-5642-8071-EB1356541E8F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -1453,47 +1424,47 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>